<commit_message>
atm swap rate added
</commit_message>
<xml_diff>
--- a/Input/Runfiles/Pricing/fixedlegs.xlsx
+++ b/Input/Runfiles/Pricing/fixedlegs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JQ228YH\Documents\CVA Tool Python\CVA-Tool\Runfiles\Pricing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JQ228YH\Documents\CVA Tool Python\CVA-Tool\Input\Runfiles\Pricing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A87A563-D8A8-4DCA-AAF4-724036B47FAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C29B52C-8328-4914-8138-0E3BD9B87CFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{52CF6CF3-B954-4931-B2B0-A068B0EE93D2}"/>
+    <workbookView xWindow="-28920" yWindow="-6465" windowWidth="29040" windowHeight="15840" xr2:uid="{52CF6CF3-B954-4931-B2B0-A068B0EE93D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <author>Vincent Verelst</author>
   </authors>
   <commentList>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{B86FB06F-0C56-412B-97F2-36271A809309}">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{B86FB06F-0C56-412B-97F2-36271A809309}">
       <text>
         <r>
           <rPr>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Dates</t>
   </si>
@@ -85,144 +85,81 @@
     <t>domestic</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>weekly</t>
   </si>
   <si>
     <t>foreign1</t>
   </si>
   <si>
-    <t>domfor1</t>
-  </si>
-  <si>
     <t>monthly</t>
   </si>
   <si>
     <t>foreign2</t>
   </si>
   <si>
-    <t>domfor2</t>
-  </si>
-  <si>
     <t>quarterly</t>
   </si>
   <si>
     <t>foreign3</t>
   </si>
   <si>
-    <t>domfor3</t>
-  </si>
-  <si>
     <t>semi-annual</t>
   </si>
   <si>
     <t>foreign4</t>
   </si>
   <si>
-    <t>domfor4</t>
-  </si>
-  <si>
     <t>annual</t>
   </si>
   <si>
     <t>foreign5</t>
   </si>
   <si>
-    <t>domfor5</t>
-  </si>
-  <si>
     <t>foreign6</t>
   </si>
   <si>
-    <t>domfor6</t>
-  </si>
-  <si>
     <t>foreign7</t>
   </si>
   <si>
-    <t>domfor7</t>
-  </si>
-  <si>
     <t>foreign8</t>
   </si>
   <si>
-    <t>domfor8</t>
-  </si>
-  <si>
     <t>foreign9</t>
   </si>
   <si>
-    <t>domfor9</t>
-  </si>
-  <si>
     <t>foreign10</t>
   </si>
   <si>
-    <t>domfor10</t>
-  </si>
-  <si>
     <t>foreign11</t>
   </si>
   <si>
-    <t>domfor11</t>
-  </si>
-  <si>
     <t>foreign12</t>
   </si>
   <si>
-    <t>domfor12</t>
-  </si>
-  <si>
     <t>foreign13</t>
   </si>
   <si>
-    <t>domfor13</t>
-  </si>
-  <si>
     <t>foreign14</t>
   </si>
   <si>
-    <t>domfor14</t>
-  </si>
-  <si>
     <t>foreign15</t>
   </si>
   <si>
-    <t>domfor15</t>
-  </si>
-  <si>
     <t>foreign16</t>
   </si>
   <si>
-    <t>domfor16</t>
-  </si>
-  <si>
     <t>foreign17</t>
   </si>
   <si>
-    <t>domfor17</t>
-  </si>
-  <si>
     <t>foreign18</t>
   </si>
   <si>
-    <t>domfor18</t>
-  </si>
-  <si>
     <t>foreign19</t>
   </si>
   <si>
-    <t>domfor19</t>
-  </si>
-  <si>
     <t>foreign20</t>
   </si>
   <si>
-    <t>domfor20</t>
-  </si>
-  <si>
     <t>Run</t>
   </si>
   <si>
@@ -238,9 +175,6 @@
     <t>Currency</t>
   </si>
   <si>
-    <t>FX</t>
-  </si>
-  <si>
     <t>Freq</t>
   </si>
   <si>
@@ -269,6 +203,15 @@
   </si>
   <si>
     <t>testamortizing</t>
+  </si>
+  <si>
+    <t>NotionalExchangeEnd</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -776,7 +719,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -785,9 +728,8 @@
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" customWidth="1"/>
-    <col min="7" max="8" width="9.88671875" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="6" max="7" width="9.88671875" customWidth="1"/>
+    <col min="8" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -829,43 +771,43 @@
     </row>
     <row r="3" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -884,23 +826,23 @@
       <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="8">
+      <c r="F4" s="8">
         <v>0.5</v>
       </c>
-      <c r="H4" s="10">
+      <c r="G4" s="10">
         <v>3.0300000000000001E-2</v>
       </c>
+      <c r="H4" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="I4" s="11" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="L4" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1281,11 +1223,11 @@
           </x14:formula1>
           <xm:sqref>E4:E44</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{70CF901B-F51A-45EF-BAA9-83EAC3DE1E95}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{278A5CFA-8592-4026-B0A7-6971C9037AF5}">
           <x14:formula1>
-            <xm:f>Sheet2!$E$1:$E$21</xm:f>
+            <xm:f>Sheet2!$E$1:$E$2</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F44</xm:sqref>
+          <xm:sqref>I4:I35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1298,7 +1240,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1311,182 +1253,125 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>